<commit_message>
webTablesTest, add, switch, rownum, search
</commit_message>
<xml_diff>
--- a/DemoQAProject.xlsx
+++ b/DemoQAProject.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B0AD43-BE7C-4205-ADC4-F61B590971B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4528792F-D612-468B-8F39-A4120C656DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="3750" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="3495" windowWidth="18000" windowHeight="9360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
     <sheet name="CheckBox" sheetId="8" r:id="rId2"/>
     <sheet name="TextBox" sheetId="2" r:id="rId3"/>
     <sheet name="RadioButton" sheetId="3" r:id="rId4"/>
-    <sheet name="Buttons" sheetId="6" r:id="rId5"/>
-    <sheet name="Alerts" sheetId="7" r:id="rId6"/>
+    <sheet name="WebTables" sheetId="9" r:id="rId5"/>
+    <sheet name="Buttons" sheetId="6" r:id="rId6"/>
+    <sheet name="Alerts" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Home</t>
   </si>
@@ -134,6 +135,44 @@
   </si>
   <si>
     <t xml:space="preserve"> commands</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Nocars</t>
+  </si>
+  <si>
+    <t>johnnocars@gmail.com</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>John
+Nocars
+23
+johnnocars@gmail.com
+234555
+Marketing</t>
   </si>
 </sst>
 </file>
@@ -703,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -732,6 +771,76 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529A89C6-BE52-48D8-81D0-DEFC9BA30C80}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1">
+        <v>234000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{7C23BE55-98C1-4DD9-9ECC-4068D12E8F52}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -773,7 +882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
invalid credential login test
</commit_message>
<xml_diff>
--- a/DemoQAProject.xlsx
+++ b/DemoQAProject.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E70433-D368-4180-97A4-45D343338AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1158C778-CB36-4C7C-B716-6008123501AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,15 @@
     <sheet name="Links" sheetId="10" r:id="rId7"/>
     <sheet name="BookStoreRegister" sheetId="11" r:id="rId8"/>
     <sheet name="BookStoreLogin" sheetId="12" r:id="rId9"/>
-    <sheet name="Alerts" sheetId="7" r:id="rId10"/>
+    <sheet name="BookStoreInvalidLogin" sheetId="13" r:id="rId10"/>
+    <sheet name="Alerts" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>Home</t>
   </si>
@@ -225,12 +226,39 @@
   <si>
     <t>Jedandva12!</t>
   </si>
+  <si>
+    <t>Invalid username</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
+  </si>
+  <si>
+    <t>JOHAN1235</t>
+  </si>
+  <si>
+    <t>Error message</t>
+  </si>
+  <si>
+    <t>Invalid username or password!</t>
+  </si>
+  <si>
+    <t>JEDANdva12!</t>
+  </si>
+  <si>
+    <t>Jedan1dva2!</t>
+  </si>
+  <si>
+    <t>jedandva123!</t>
+  </si>
+  <si>
+    <t>johan1235</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,13 +282,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,11 +312,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -287,9 +328,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,6 +711,71 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6190F9C7-8CB1-4E48-85D2-0C91FA8AA830}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1101,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7772EA20-D1C3-4C5E-80AC-486F8CDB1CBD}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>